<commit_message>
Implementado sistema de login completo con localStorage y tests
</commit_message>
<xml_diff>
--- a/excel/PROMOCIONES.xlsx
+++ b/excel/PROMOCIONES.xlsx
@@ -49,6 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,7 +83,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,7 +367,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,7 +375,7 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -386,7 +389,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -412,5 +415,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eliminar decimales en precios de artículos para mejorar la visualización de datos en JSON
</commit_message>
<xml_diff>
--- a/excel/PROMOCIONES.xlsx
+++ b/excel/PROMOCIONES.xlsx
@@ -369,7 +369,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +402,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>432</v>
+        <v>432.24099999999999</v>
       </c>
       <c r="D2" s="1">
         <v>45657</v>

</xml_diff>